<commit_message>
G3WS-12 Adicionando o envio de anexo (planilha excel)
</commit_message>
<xml_diff>
--- a/PlanilhaListaVulnerabilidades.xlsx
+++ b/PlanilhaListaVulnerabilidades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://facens-my.sharepoint.com/personal/gelson_filho_facens_br/Documents/Documentos/Desafios Lenovo-FACENS/Desafio 1 - WebScraping/Repositorio_Desafio_1/G3WP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive - Centro Universitário Facens\Documentos\Desafios Lenovo-FACENS\Desafio 1 - WebScraping\Repositorio_Desafio_1\G3WP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F92581B-22EE-4985-A9B5-8F857458E54C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{2F92581B-22EE-4985-A9B5-8F857458E54C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8752329C-8226-4FC8-9518-702BD4DE53A8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{4BD3F848-DCF6-4677-919D-79738040FD22}"/>
   </bookViews>
@@ -22,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+  <si>
+    <t>a</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,17 +379,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37AF5A7-3CAD-4D36-9892-98B32D1A18AC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004260A06BB74F5B4693D338ED5E2BFB8F" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4ffece7e6cfc7dd6a64827fed49996ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd804457-e93e-4ad8-a44a-f200675f42df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed0ca48688166084165afc31c93e5de6" ns3:_="">
     <xsd:import namespace="cd804457-e93e-4ad8-a44a-f200675f42df"/>
@@ -539,22 +579,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41CE57E0-0561-4F5A-8699-DB7EFE8B6CC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cd804457-e93e-4ad8-a44a-f200675f42df"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05DFE78-B700-49AC-A2F4-BC46CB16AC7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378C7166-E516-4576-8E30-7AC860B3C1D5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -570,28 +619,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05DFE78-B700-49AC-A2F4-BC46CB16AC7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41CE57E0-0561-4F5A-8699-DB7EFE8B6CC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="cd804457-e93e-4ad8-a44a-f200675f42df"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
G3WS-12 Alterações pontuais de teste, acréscimo de mais destinatários de email e tirando a biblioteca pandas do codigo principal
</commit_message>
<xml_diff>
--- a/PlanilhaListaVulnerabilidades.xlsx
+++ b/PlanilhaListaVulnerabilidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive - Centro Universitário Facens\Documentos\Desafios Lenovo-FACENS\Desafio 1 - WebScraping\Repositorio_Desafio_1\G3WP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{2F92581B-22EE-4985-A9B5-8F857458E54C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8752329C-8226-4FC8-9518-702BD4DE53A8}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{2F92581B-22EE-4985-A9B5-8F857458E54C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{8CB0C452-BBCF-464B-826A-8393BB4664A2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{4BD3F848-DCF6-4677-919D-79738040FD22}"/>
   </bookViews>
@@ -25,16 +25,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
-  <si>
-    <t>a</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="26">
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>CVE</t>
+  </si>
+  <si>
+    <t>Current Description</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>References to Advisories	 Solutions	 and Tools</t>
+  </si>
+  <si>
+    <t>Known Affected Software Configurations</t>
+  </si>
+  <si>
+    <t>NVD Published Date</t>
+  </si>
+  <si>
+    <t>Link para o respectivo CVE</t>
+  </si>
+  <si>
+    <t>log4J</t>
+  </si>
+  <si>
+    <t>CVE-2022-0070</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>04/19/2022</t>
+  </si>
+  <si>
+    <t>https://google.com</t>
+  </si>
+  <si>
+    <t>CVE-2022-0071</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>04/19/2023</t>
+  </si>
+  <si>
+    <t>CVE-2022-0072</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>04/19/2024</t>
+  </si>
+  <si>
+    <t>CVE-2022-0073</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>04/19/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +117,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -59,12 +154,192 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,49 +654,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37AF5A7-3CAD-4D36-9892-98B32D1A18AC}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004260A06BB74F5B4693D338ED5E2BFB8F" ma:contentTypeVersion="6" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="4ffece7e6cfc7dd6a64827fed49996ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd804457-e93e-4ad8-a44a-f200675f42df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed0ca48688166084165afc31c93e5de6" ns3:_="">
     <xsd:import namespace="cd804457-e93e-4ad8-a44a-f200675f42df"/>
@@ -579,31 +966,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41CE57E0-0561-4F5A-8699-DB7EFE8B6CC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cd804457-e93e-4ad8-a44a-f200675f42df"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05DFE78-B700-49AC-A2F4-BC46CB16AC7B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{378C7166-E516-4576-8E30-7AC860B3C1D5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -619,4 +997,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C05DFE78-B700-49AC-A2F4-BC46CB16AC7B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41CE57E0-0561-4F5A-8699-DB7EFE8B6CC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="cd804457-e93e-4ad8-a44a-f200675f42df"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>